<commit_message>
Publish Project On Host
</commit_message>
<xml_diff>
--- a/امور پرسنلی/مهندس بقایی/کارکرد مهندس بقایی.xlsx
+++ b/امور پرسنلی/مهندس بقایی/کارکرد مهندس بقایی.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="55">
   <si>
     <t>نوع فعالیت</t>
   </si>
@@ -179,6 +179,12 @@
   </si>
   <si>
     <t>تفکیکو تغییر لایه بندی پروژه به 7 لایه و اضافه شدن لایه ViewModels</t>
+  </si>
+  <si>
+    <t>پابلیش پروژه روی هاست و حل باگ های موجود روی swagger و Nlog</t>
+  </si>
+  <si>
+    <t>1399/09/02</t>
   </si>
 </sst>
 </file>
@@ -893,8 +899,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E130"/>
   <sheetViews>
-    <sheetView rightToLeft="1" tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+    <sheetView rightToLeft="1" tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.45"/>
@@ -1247,7 +1253,18 @@
       <c r="E23" s="8"/>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A24" s="8"/>
+      <c r="A24" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="B24" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="C24" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="D24" s="8">
+        <v>9</v>
+      </c>
       <c r="E24" s="8"/>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.45">

</xml_diff>

<commit_message>
Work For Deleted Project
</commit_message>
<xml_diff>
--- a/امور پرسنلی/مهندس بقایی/کارکرد مهندس بقایی.xlsx
+++ b/امور پرسنلی/مهندس بقایی/کارکرد مهندس بقایی.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="57">
   <si>
     <t>نوع فعالیت</t>
   </si>
@@ -178,13 +178,19 @@
     <t>1399/08/27</t>
   </si>
   <si>
-    <t>تفکیکو تغییر لایه بندی پروژه به 7 لایه و اضافه شدن لایه ViewModels</t>
-  </si>
-  <si>
-    <t>پابلیش پروژه روی هاست و حل باگ های موجود روی swagger و Nlog</t>
-  </si>
-  <si>
     <t>1399/09/02</t>
+  </si>
+  <si>
+    <t>حذف شدن پروژه و نوشتن کدهای برنامه از اول</t>
+  </si>
+  <si>
+    <t>1399/09/01</t>
+  </si>
+  <si>
+    <t>تفکیک و تغییر لایه بندی پروژه به 7 لایه و اضافه شدن لایه ViewModels</t>
+  </si>
+  <si>
+    <t>پابلیش پروژه روی هاست و حل باگ های موجود روی swagger و Nlog و خطاهای روی آپدیت و حذف رکورد از بانک</t>
   </si>
 </sst>
 </file>
@@ -899,8 +905,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E130"/>
   <sheetViews>
-    <sheetView rightToLeft="1" tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+    <sheetView rightToLeft="1" tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.45"/>
@@ -1237,12 +1243,12 @@
       </c>
       <c r="E22" s="8"/>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:5" ht="37.5" x14ac:dyDescent="0.45">
       <c r="A23" s="8" t="s">
         <v>22</v>
       </c>
       <c r="B23" s="7" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="C23" s="8" t="s">
         <v>51</v>
@@ -1263,12 +1269,23 @@
         <v>54</v>
       </c>
       <c r="D24" s="8">
+        <v>0</v>
+      </c>
+      <c r="E24" s="8"/>
+    </row>
+    <row r="25" spans="1:5" ht="37.5" x14ac:dyDescent="0.45">
+      <c r="A25" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="B25" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="C25" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="D25" s="8">
         <v>9</v>
       </c>
-      <c r="E24" s="8"/>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A25" s="8"/>
       <c r="E25" s="8"/>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.45">
@@ -1604,7 +1621,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
   <tableParts count="1">
     <tablePart r:id="rId2"/>
   </tableParts>

</xml_diff>

<commit_message>
Create Vuenative Mobile App
</commit_message>
<xml_diff>
--- a/امور پرسنلی/مهندس بقایی/کارکرد مهندس بقایی.xlsx
+++ b/امور پرسنلی/مهندس بقایی/کارکرد مهندس بقایی.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="59">
   <si>
     <t>نوع فعالیت</t>
   </si>
@@ -191,6 +191,12 @@
   </si>
   <si>
     <t>پابلیش پروژه روی هاست و حل باگ های موجود روی swagger و Nlog و خطاهای روی آپدیت و حذف رکورد از بانک</t>
+  </si>
+  <si>
+    <t>1399/09/03</t>
+  </si>
+  <si>
+    <t>ایجاد اپ موبایل با React-native و تبدیل به Vue-native و تنظیمات و کدنویسی زیرساخت پروژه و بکاپ گیری از تمامی پروژه ها روی سیستم ویرا و لب تاپ و فلش</t>
   </si>
 </sst>
 </file>
@@ -906,7 +912,7 @@
   <dimension ref="A1:E130"/>
   <sheetViews>
     <sheetView rightToLeft="1" tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+      <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.45"/>
@@ -1288,8 +1294,19 @@
       </c>
       <c r="E25" s="8"/>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A26" s="8"/>
+    <row r="26" spans="1:5" ht="56.25" x14ac:dyDescent="0.45">
+      <c r="A26" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="B26" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="C26" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="D26" s="8">
+        <v>4</v>
+      </c>
       <c r="E26" s="8"/>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.45">

</xml_diff>